<commit_message>
chore(import): simplify payout import to use model code only (remove name columns); update template and add test
</commit_message>
<xml_diff>
--- a/app/static/import_templates/payroll_import_template.xlsx
+++ b/app/static/import_templates/payroll_import_template.xlsx
@@ -578,7 +578,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -619,16 +619,6 @@
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Working Name</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Real Name</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
           <t>Notes</t>
         </is>
       </c>
@@ -664,16 +654,6 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Janie D</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>Jane Doe</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
           <t>June retainer</t>
         </is>
       </c>
@@ -709,16 +689,6 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>AK</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>Alicia Keys</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
           <t>Campaign launch</t>
         </is>
       </c>
@@ -753,16 +723,6 @@
         </is>
       </c>
       <c r="G4" t="inlineStr">
-        <is>
-          <t>AK</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>Alicia Keys</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
         <is>
           <t>Adjusted schedule</t>
         </is>

</xml_diff>